<commit_message>
Fixed bug --end flag ingnored
</commit_message>
<xml_diff>
--- a/examples/example1.xlsx
+++ b/examples/example1.xlsx
@@ -384,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,6 +412,22 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1485938350</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1485938350</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>